<commit_message>
Modified database add new 17 Controller
</commit_message>
<xml_diff>
--- a/RatingUniversity/Files/15_effektivnost_nir.xlsx
+++ b/RatingUniversity/Files/15_effektivnost_nir.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repositories\Raiting\RatingUniversity\Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
@@ -102,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -329,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -381,6 +386,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,25 +419,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -689,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -716,77 +727,77 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="27"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -888,77 +899,77 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="27"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1043,7 +1054,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1059,93 +1070,105 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="27"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="11">
         <v>1</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="11"/>
+      <c r="B8" s="11">
+        <v>2</v>
+      </c>
+      <c r="C8" s="31">
+        <v>3</v>
+      </c>
+      <c r="D8" s="31">
+        <v>4</v>
+      </c>
+      <c r="E8" s="31">
+        <v>5</v>
+      </c>
+      <c r="F8" s="32">
+        <v>6</v>
+      </c>
+      <c r="G8" s="11">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">

</xml_diff>